<commit_message>
Keywords now disappear from guidebook when leaving interact rings
</commit_message>
<xml_diff>
--- a/All Examples Data.xlsx
+++ b/All Examples Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\FYP-3 - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653B3DC6-22B2-4F3B-BA18-0E50F3C1AF35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F985C-E613-4F27-A83B-8A7CABF73BB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="5190" windowWidth="13170" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4627" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4737" uniqueCount="1107">
   <si>
     <t>Version</t>
   </si>
@@ -4233,10 +4233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H140"/>
+  <dimension ref="A1:H162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="G134" sqref="G134"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="H146" sqref="H146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6215,427 +6215,801 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
-        <v>440</v>
-      </c>
-      <c r="B116" s="18" t="s">
-        <v>448</v>
-      </c>
-      <c r="C116" s="18" t="s">
-        <v>448</v>
-      </c>
-      <c r="D116" s="18" t="s">
-        <v>449</v>
-      </c>
-      <c r="E116" s="19" t="s">
-        <v>1082</v>
+      <c r="A116" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>582</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>448</v>
+      <c r="A117" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="E117" s="21" t="s">
-        <v>1088</v>
+        <v>1078</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B118" s="1" t="s">
-        <v>448</v>
+      <c r="A118" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E118" s="21" t="s">
-        <v>1083</v>
+        <v>1079</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>586</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>448</v>
+      <c r="A119" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E119" s="21" t="s">
-        <v>1084</v>
+        <v>1080</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B120" s="1" t="s">
-        <v>448</v>
+      <c r="A120" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E120" s="21" t="s">
-        <v>1085</v>
+        <v>590</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>448</v>
+      <c r="A121" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="E121" s="21" t="s">
-        <v>1086</v>
+        <v>477</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>592</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B122" s="1" t="s">
-        <v>448</v>
+      <c r="A122" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="E122" s="21" t="s">
-        <v>1087</v>
+        <v>479</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>593</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B123" s="1" t="s">
-        <v>448</v>
+      <c r="A123" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E123" s="21" t="s">
-        <v>1094</v>
+        <v>481</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>594</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B124" s="1" t="s">
-        <v>448</v>
+      <c r="A124" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E124" s="21" t="s">
-        <v>1095</v>
+        <v>483</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B125" s="1" t="s">
-        <v>448</v>
+      <c r="A125" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1091</v>
-      </c>
-      <c r="E125" s="21" t="s">
-        <v>1096</v>
+        <v>485</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B126" s="1" t="s">
-        <v>448</v>
+      <c r="A126" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1092</v>
-      </c>
-      <c r="E126" s="21" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>448</v>
+        <v>8</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E127" s="21" t="s">
-        <v>1098</v>
+        <v>1078</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B128" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="D128" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="E128" s="5" t="s">
-        <v>1082</v>
+      <c r="B128" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B129" s="1" t="s">
-        <v>448</v>
+      <c r="B129" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>457</v>
+        <v>1080</v>
       </c>
       <c r="E129" s="7" t="s">
-        <v>1088</v>
+        <v>599</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B130" s="1" t="s">
-        <v>448</v>
+      <c r="B130" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>460</v>
+        <v>1081</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>1085</v>
+        <v>600</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>448</v>
+      <c r="B131" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>460</v>
+        <v>477</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>1086</v>
+        <v>601</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>448</v>
+      <c r="B132" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>464</v>
+        <v>479</v>
       </c>
       <c r="E132" s="7" t="s">
-        <v>1087</v>
+        <v>602</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>448</v>
+      <c r="B133" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1089</v>
+        <v>481</v>
       </c>
       <c r="E133" s="7" t="s">
-        <v>1094</v>
+        <v>603</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B134" s="1" t="s">
-        <v>448</v>
+      <c r="B134" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1090</v>
+        <v>483</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>1095</v>
+        <v>604</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>448</v>
+      <c r="B135" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1091</v>
+        <v>485</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>1096</v>
+        <v>605</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>448</v>
+      <c r="B136" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1092</v>
+        <v>13</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>1097</v>
+        <v>606</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
         <v>1049</v>
       </c>
-      <c r="B137" s="9" t="s">
-        <v>448</v>
+      <c r="B137" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>448</v>
+        <v>30</v>
       </c>
       <c r="D137" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E137" s="10" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="17" t="s">
+        <v>440</v>
+      </c>
+      <c r="B138" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="C138" s="18" t="s">
+        <v>448</v>
+      </c>
+      <c r="D138" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="E138" s="19" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E139" s="21" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E140" s="21" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="E141" s="21" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E142" s="21" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E143" s="21" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E144" s="21" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E145" s="21" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E146" s="21" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E147" s="21" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E148" s="21" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="20" t="s">
+        <v>440</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D149" s="1" t="s">
         <v>1093</v>
       </c>
-      <c r="E137" s="10" t="s">
+      <c r="E149" s="21" t="s">
         <v>1098</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="3" t="s">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
         <v>1049</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B150" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D152" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D153" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="E154" s="7" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E156" s="7" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>1092</v>
+      </c>
+      <c r="E158" s="7" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="8" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E159" s="10" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B160" s="4" t="s">
         <v>1099</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C160" s="4" t="s">
         <v>1100</v>
       </c>
-      <c r="D138" s="4" t="s">
+      <c r="D160" s="4" t="s">
         <v>1101</v>
       </c>
-      <c r="E138" s="5" t="s">
+      <c r="E160" s="5" t="s">
         <v>1102</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="6" t="s">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="6" t="s">
         <v>1049</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B161" s="1" t="s">
         <v>1099</v>
       </c>
-      <c r="C139" s="1" t="s">
+      <c r="C161" s="1" t="s">
         <v>1100</v>
       </c>
-      <c r="D139" s="1" t="s">
+      <c r="D161" s="1" t="s">
         <v>1103</v>
       </c>
-      <c r="E139" s="7" t="s">
+      <c r="E161" s="7" t="s">
         <v>1104</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="8" t="s">
+    <row r="162" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A162" s="8" t="s">
         <v>1049</v>
       </c>
-      <c r="B140" s="9" t="s">
+      <c r="B162" s="9" t="s">
         <v>1099</v>
       </c>
-      <c r="C140" s="9" t="s">
+      <c r="C162" s="9" t="s">
         <v>1100</v>
       </c>
-      <c r="D140" s="9" t="s">
+      <c r="D162" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="E140" s="10" t="s">
+      <c r="E162" s="10" t="s">
         <v>1106</v>
       </c>
     </row>

</xml_diff>